<commit_message>
nuevo metodo de superior en memoria
</commit_message>
<xml_diff>
--- a/src/main/resources/superior.xlsx
+++ b/src/main/resources/superior.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariano\Documents\NetBeansProjects\SpringMECApiV1\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ledes\Documents\NetBeansProjects\SpringMECApiV1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -279,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +289,13 @@
     </font>
     <font>
       <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="PT Sans"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="PT Sans"/>
@@ -348,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -365,12 +372,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -383,10 +384,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,20 +671,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B330"/>
+  <dimension ref="A1:B328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="A326" sqref="A326:B328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8">
+      <c r="A1" s="6">
         <v>180141900</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -688,7 +692,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>180176400</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -696,7 +700,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>180176400</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -704,7 +708,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>180176400</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -712,7 +716,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>180176400</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -720,7 +724,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>180176400</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -728,7 +732,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>180176400</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -736,7 +740,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>180176400</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -744,7 +748,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>180141900</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -752,7 +756,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>180141900</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -760,7 +764,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>180141900</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -768,7 +772,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>180141900</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -776,7 +780,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>180141900</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -784,7 +788,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>180141900</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -792,7 +796,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>180141900</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -800,7 +804,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>180141900</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -808,7 +812,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>180141900</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -816,7 +820,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="8">
+      <c r="A18" s="6">
         <v>180141900</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -824,7 +828,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>180141900</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -832,7 +836,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>180141900</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -840,7 +844,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>180141900</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -848,7 +852,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="8">
+      <c r="A22" s="6">
         <v>180141900</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -856,7 +860,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>180141900</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -864,7 +868,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="8">
+      <c r="A24" s="6">
         <v>180141900</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -872,7 +876,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="8">
+      <c r="A25" s="6">
         <v>180081502</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -880,7 +884,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="8">
+      <c r="A26" s="6">
         <v>180176500</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -888,7 +892,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="8">
+      <c r="A27" s="6">
         <v>180176500</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -896,7 +900,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="8">
+      <c r="A28" s="6">
         <v>180176500</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -904,7 +908,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="8">
+      <c r="A29" s="6">
         <v>180176500</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -912,7 +916,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="8">
+      <c r="A30" s="6">
         <v>180117600</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -920,7 +924,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="8">
+      <c r="A31" s="6">
         <v>180117600</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -928,7 +932,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="8">
+      <c r="A32" s="6">
         <v>180117600</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -936,7 +940,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="8">
+      <c r="A33" s="6">
         <v>180117600</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -944,7 +948,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="8">
+      <c r="A34" s="6">
         <v>180117600</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -952,7 +956,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="8">
+      <c r="A35" s="6">
         <v>180117600</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -960,7 +964,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="8">
+      <c r="A36" s="6">
         <v>180117600</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -968,7 +972,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="8">
+      <c r="A37" s="6">
         <v>180117600</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -976,7 +980,7 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="8">
+      <c r="A38" s="6">
         <v>180173000</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -984,7 +988,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="8">
+      <c r="A39" s="6">
         <v>180114500</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -992,7 +996,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="8">
+      <c r="A40" s="6">
         <v>180114500</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1000,7 +1004,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="8">
+      <c r="A41" s="6">
         <v>180114500</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1008,7 +1012,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="8">
+      <c r="A42" s="6">
         <v>180114500</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1016,7 +1020,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="8">
+      <c r="A43" s="6">
         <v>180114500</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1024,7 +1028,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="8">
+      <c r="A44" s="6">
         <v>180114500</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1032,7 +1036,7 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="8">
+      <c r="A45" s="6">
         <v>180114500</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1040,7 +1044,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="8">
+      <c r="A46" s="6">
         <v>180063400</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1048,7 +1052,7 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="8">
+      <c r="A47" s="6">
         <v>180081500</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1056,7 +1060,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="8">
+      <c r="A48" s="6">
         <v>180081500</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1064,7 +1068,7 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="8">
+      <c r="A49" s="6">
         <v>180081500</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1072,7 +1076,7 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="8">
+      <c r="A50" s="6">
         <v>180081500</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1080,7 +1084,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="8">
+      <c r="A51" s="6">
         <v>180081500</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1088,7 +1092,7 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="8">
+      <c r="A52" s="6">
         <v>180081500</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1096,7 +1100,7 @@
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="8">
+      <c r="A53" s="6">
         <v>180081500</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1104,7 +1108,7 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="8">
+      <c r="A54" s="6">
         <v>180141100</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1112,7 +1116,7 @@
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="8">
+      <c r="A55" s="6">
         <v>180141100</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1120,7 +1124,7 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="8">
+      <c r="A56" s="6">
         <v>180141100</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1128,7 +1132,7 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="8">
+      <c r="A57" s="6">
         <v>180141100</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1136,7 +1140,7 @@
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="8">
+      <c r="A58" s="6">
         <v>180141100</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1144,7 +1148,7 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="8">
+      <c r="A59" s="6">
         <v>180141100</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1152,7 +1156,7 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="8">
+      <c r="A60" s="6">
         <v>180141200</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1160,7 +1164,7 @@
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="8">
+      <c r="A61" s="6">
         <v>180141200</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1168,7 +1172,7 @@
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="8">
+      <c r="A62" s="6">
         <v>180141200</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1176,7 +1180,7 @@
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="8">
+      <c r="A63" s="6">
         <v>180141200</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1184,7 +1188,7 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="8">
+      <c r="A64" s="6">
         <v>180141200</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1192,7 +1196,7 @@
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="8">
+      <c r="A65" s="6">
         <v>180141200</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1200,7 +1204,7 @@
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="8">
+      <c r="A66" s="6">
         <v>180165000</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1208,7 +1212,7 @@
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="8">
+      <c r="A67" s="6">
         <v>180165000</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1216,7 +1220,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="8">
+      <c r="A68" s="6">
         <v>180165000</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1224,7 +1228,7 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="8">
+      <c r="A69" s="6">
         <v>180164600</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1232,7 +1236,7 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="8">
+      <c r="A70" s="6">
         <v>180164600</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1240,7 +1244,7 @@
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="8">
+      <c r="A71" s="6">
         <v>180164600</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -1248,7 +1252,7 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="8">
+      <c r="A72" s="6">
         <v>180164600</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1256,7 +1260,7 @@
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="8">
+      <c r="A73" s="6">
         <v>180041100</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1264,7 +1268,7 @@
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="8">
+      <c r="A74" s="6">
         <v>180041100</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -1272,7 +1276,7 @@
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="8">
+      <c r="A75" s="6">
         <v>180041100</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -1280,7 +1284,7 @@
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="8">
+      <c r="A76" s="6">
         <v>180041100</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1288,7 +1292,7 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="8">
+      <c r="A77" s="6">
         <v>180146603</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1296,7 +1300,7 @@
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="8">
+      <c r="A78" s="6">
         <v>180146603</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1304,7 +1308,7 @@
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="8">
+      <c r="A79" s="6">
         <v>180142600</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1312,7 +1316,7 @@
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="8">
+      <c r="A80" s="6">
         <v>180142600</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -1320,7 +1324,7 @@
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="8">
+      <c r="A81" s="6">
         <v>180121801</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -1328,7 +1332,7 @@
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="8">
+      <c r="A82" s="6">
         <v>180121801</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -1336,7 +1340,7 @@
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="8">
+      <c r="A83" s="6">
         <v>180177300</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -1344,7 +1348,7 @@
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="8">
+      <c r="A84" s="6">
         <v>180141203</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -1352,7 +1356,7 @@
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="8">
+      <c r="A85" s="6">
         <v>180141203</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -1360,7 +1364,7 @@
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="8">
+      <c r="A86" s="6">
         <v>180177301</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -1368,7 +1372,7 @@
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="8">
+      <c r="A87" s="6">
         <v>180177300</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -1376,7 +1380,7 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="8">
+      <c r="A88" s="6">
         <v>180177301</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -1384,7 +1388,7 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="8">
+      <c r="A89" s="6">
         <v>180067500</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -1392,7 +1396,7 @@
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="8">
+      <c r="A90" s="6">
         <v>180067500</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -1400,7 +1404,7 @@
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="8">
+      <c r="A91" s="6">
         <v>180067500</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -1408,7 +1412,7 @@
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="8">
+      <c r="A92" s="6">
         <v>180067500</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -1416,7 +1420,7 @@
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="8">
+      <c r="A93" s="6">
         <v>180067500</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -1424,7 +1428,7 @@
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="8">
+      <c r="A94" s="6">
         <v>180067500</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -1432,7 +1436,7 @@
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="8">
+      <c r="A95" s="6">
         <v>180067500</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -1440,7 +1444,7 @@
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="8">
+      <c r="A96" s="6">
         <v>180067500</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -1448,7 +1452,7 @@
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="8">
+      <c r="A97" s="6">
         <v>180067500</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -1456,7 +1460,7 @@
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="8">
+      <c r="A98" s="6">
         <v>180067500</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -1464,7 +1468,7 @@
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="8">
+      <c r="A99" s="6">
         <v>180165000</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -1472,7 +1476,7 @@
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="8">
+      <c r="A100" s="6">
         <v>180165000</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -1480,7 +1484,7 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="8">
+      <c r="A101" s="6">
         <v>180145100</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -1488,7 +1492,7 @@
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="8">
+      <c r="A102" s="6">
         <v>180145100</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -1496,7 +1500,7 @@
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="8">
+      <c r="A103" s="6">
         <v>180145100</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -1504,7 +1508,7 @@
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="8">
+      <c r="A104" s="6">
         <v>180145100</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -1512,7 +1516,7 @@
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="8">
+      <c r="A105" s="6">
         <v>180145100</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -1520,7 +1524,7 @@
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="8">
+      <c r="A106" s="6">
         <v>180141300</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -1528,7 +1532,7 @@
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="8">
+      <c r="A107" s="6">
         <v>180141300</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -1536,7 +1540,7 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="8">
+      <c r="A108" s="6">
         <v>180141300</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -1544,7 +1548,7 @@
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="8">
+      <c r="A109" s="6">
         <v>180141300</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -1552,7 +1556,7 @@
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="8">
+      <c r="A110" s="6">
         <v>180141300</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -1560,7 +1564,7 @@
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="8">
+      <c r="A111" s="6">
         <v>180141300</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -1568,7 +1572,7 @@
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="8">
+      <c r="A112" s="6">
         <v>180141300</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -1576,7 +1580,7 @@
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="8">
+      <c r="A113" s="6">
         <v>180146601</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -1584,7 +1588,7 @@
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="8">
+      <c r="A114" s="6">
         <v>180146601</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -1592,7 +1596,7 @@
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="8">
+      <c r="A115" s="6">
         <v>180146601</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -1600,7 +1604,7 @@
       </c>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="8">
+      <c r="A116" s="6">
         <v>180121800</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -1608,7 +1612,7 @@
       </c>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="8">
+      <c r="A117" s="6">
         <v>180121800</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -1616,7 +1620,7 @@
       </c>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="8">
+      <c r="A118" s="6">
         <v>180121800</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -1624,7 +1628,7 @@
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="8">
+      <c r="A119" s="6">
         <v>180121800</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -1632,7 +1636,7 @@
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="8">
+      <c r="A120" s="6">
         <v>180121800</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -1640,7 +1644,7 @@
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="8">
+      <c r="A121" s="6">
         <v>180121800</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -1648,7 +1652,7 @@
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="8">
+      <c r="A122" s="6">
         <v>180121800</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -1656,7 +1660,7 @@
       </c>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="8">
+      <c r="A123" s="6">
         <v>180142600</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -1664,7 +1668,7 @@
       </c>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="8">
+      <c r="A124" s="6">
         <v>180142600</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -1672,7 +1676,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" ht="22.5">
-      <c r="A125" s="8">
+      <c r="A125" s="6">
         <v>180142600</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -1680,7 +1684,7 @@
       </c>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="8">
+      <c r="A126" s="6">
         <v>180142600</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -1688,7 +1692,7 @@
       </c>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="8">
+      <c r="A127" s="6">
         <v>180142600</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -1696,7 +1700,7 @@
       </c>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="8">
+      <c r="A128" s="6">
         <v>180142600</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -1704,7 +1708,7 @@
       </c>
     </row>
     <row r="129" spans="1:2">
-      <c r="A129" s="8">
+      <c r="A129" s="6">
         <v>180142600</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -1712,7 +1716,7 @@
       </c>
     </row>
     <row r="130" spans="1:2">
-      <c r="A130" s="8">
+      <c r="A130" s="6">
         <v>180142600</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -1720,7 +1724,7 @@
       </c>
     </row>
     <row r="131" spans="1:2">
-      <c r="A131" s="8">
+      <c r="A131" s="6">
         <v>180142600</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -1728,7 +1732,7 @@
       </c>
     </row>
     <row r="132" spans="1:2">
-      <c r="A132" s="8">
+      <c r="A132" s="6">
         <v>180142600</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -1736,7 +1740,7 @@
       </c>
     </row>
     <row r="133" spans="1:2">
-      <c r="A133" s="8">
+      <c r="A133" s="6">
         <v>180142600</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -1744,7 +1748,7 @@
       </c>
     </row>
     <row r="134" spans="1:2">
-      <c r="A134" s="8">
+      <c r="A134" s="6">
         <v>180142600</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -1752,7 +1756,7 @@
       </c>
     </row>
     <row r="135" spans="1:2">
-      <c r="A135" s="8">
+      <c r="A135" s="6">
         <v>180142600</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -1760,7 +1764,7 @@
       </c>
     </row>
     <row r="136" spans="1:2">
-      <c r="A136" s="8">
+      <c r="A136" s="6">
         <v>180142600</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -1768,7 +1772,7 @@
       </c>
     </row>
     <row r="137" spans="1:2">
-      <c r="A137" s="8">
+      <c r="A137" s="6">
         <v>180142600</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -1776,7 +1780,7 @@
       </c>
     </row>
     <row r="138" spans="1:2">
-      <c r="A138" s="8">
+      <c r="A138" s="6">
         <v>180142600</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -1784,7 +1788,7 @@
       </c>
     </row>
     <row r="139" spans="1:2">
-      <c r="A139" s="8">
+      <c r="A139" s="6">
         <v>180142600</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -1792,7 +1796,7 @@
       </c>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="8">
+      <c r="A140" s="6">
         <v>180142600</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -1800,7 +1804,7 @@
       </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="8">
+      <c r="A141" s="6">
         <v>180142600</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -1808,7 +1812,7 @@
       </c>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="8">
+      <c r="A142" s="6">
         <v>180142600</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -1816,7 +1820,7 @@
       </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="8">
+      <c r="A143" s="6">
         <v>180176800</v>
       </c>
       <c r="B143" s="1" t="s">
@@ -1824,7 +1828,7 @@
       </c>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="8">
+      <c r="A144" s="6">
         <v>180176800</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -1832,7 +1836,7 @@
       </c>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="8">
+      <c r="A145" s="6">
         <v>180141102</v>
       </c>
       <c r="B145" s="1" t="s">
@@ -1840,7 +1844,7 @@
       </c>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="8">
+      <c r="A146" s="6">
         <v>180141102</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -1848,7 +1852,7 @@
       </c>
     </row>
     <row r="147" spans="1:2">
-      <c r="A147" s="8">
+      <c r="A147" s="6">
         <v>180141102</v>
       </c>
       <c r="B147" s="1" t="s">
@@ -1856,7 +1860,7 @@
       </c>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" s="8">
+      <c r="A148" s="6">
         <v>180141102</v>
       </c>
       <c r="B148" s="1" t="s">
@@ -1864,7 +1868,7 @@
       </c>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="8">
+      <c r="A149" s="6">
         <v>180141102</v>
       </c>
       <c r="B149" s="1" t="s">
@@ -1872,7 +1876,7 @@
       </c>
     </row>
     <row r="150" spans="1:2">
-      <c r="A150" s="8">
+      <c r="A150" s="6">
         <v>180165004</v>
       </c>
       <c r="B150" s="1" t="s">
@@ -1880,7 +1884,7 @@
       </c>
     </row>
     <row r="151" spans="1:2">
-      <c r="A151" s="8">
+      <c r="A151" s="6">
         <v>180165004</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -1888,7 +1892,7 @@
       </c>
     </row>
     <row r="152" spans="1:2">
-      <c r="A152" s="8">
+      <c r="A152" s="6">
         <v>180141103</v>
       </c>
       <c r="B152" s="1" t="s">
@@ -1896,7 +1900,7 @@
       </c>
     </row>
     <row r="153" spans="1:2">
-      <c r="A153" s="8">
+      <c r="A153" s="6">
         <v>180141103</v>
       </c>
       <c r="B153" s="1" t="s">
@@ -1904,7 +1908,7 @@
       </c>
     </row>
     <row r="154" spans="1:2">
-      <c r="A154" s="8">
+      <c r="A154" s="6">
         <v>180182900</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -1912,7 +1916,7 @@
       </c>
     </row>
     <row r="155" spans="1:2">
-      <c r="A155" s="8">
+      <c r="A155" s="6">
         <v>180182900</v>
       </c>
       <c r="B155" s="1" t="s">
@@ -1920,7 +1924,7 @@
       </c>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="8">
+      <c r="A156" s="6">
         <v>180165001</v>
       </c>
       <c r="B156" s="1" t="s">
@@ -1928,7 +1932,7 @@
       </c>
     </row>
     <row r="157" spans="1:2">
-      <c r="A157" s="8">
+      <c r="A157" s="6">
         <v>180182900</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -1936,7 +1940,7 @@
       </c>
     </row>
     <row r="158" spans="1:2">
-      <c r="A158" s="8">
+      <c r="A158" s="6">
         <v>180182900</v>
       </c>
       <c r="B158" s="1" t="s">
@@ -1944,7 +1948,7 @@
       </c>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" s="8">
+      <c r="A159" s="6">
         <v>180176800</v>
       </c>
       <c r="B159" s="1" t="s">
@@ -1952,7 +1956,7 @@
       </c>
     </row>
     <row r="160" spans="1:2">
-      <c r="A160" s="8">
+      <c r="A160" s="6">
         <v>180176800</v>
       </c>
       <c r="B160" s="1" t="s">
@@ -1960,7 +1964,7 @@
       </c>
     </row>
     <row r="161" spans="1:2">
-      <c r="A161" s="8">
+      <c r="A161" s="6">
         <v>180176800</v>
       </c>
       <c r="B161" s="1" t="s">
@@ -1968,7 +1972,7 @@
       </c>
     </row>
     <row r="162" spans="1:2">
-      <c r="A162" s="8">
+      <c r="A162" s="6">
         <v>180176800</v>
       </c>
       <c r="B162" s="1" t="s">
@@ -1976,7 +1980,7 @@
       </c>
     </row>
     <row r="163" spans="1:2">
-      <c r="A163" s="8">
+      <c r="A163" s="6">
         <v>180176800</v>
       </c>
       <c r="B163" s="1" t="s">
@@ -1984,7 +1988,7 @@
       </c>
     </row>
     <row r="164" spans="1:2">
-      <c r="A164" s="8">
+      <c r="A164" s="6">
         <v>180176800</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -1992,7 +1996,7 @@
       </c>
     </row>
     <row r="165" spans="1:2">
-      <c r="A165" s="8">
+      <c r="A165" s="6">
         <v>180176800</v>
       </c>
       <c r="B165" s="1" t="s">
@@ -2000,7 +2004,7 @@
       </c>
     </row>
     <row r="166" spans="1:2">
-      <c r="A166" s="8">
+      <c r="A166" s="6">
         <v>180176800</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -2008,7 +2012,7 @@
       </c>
     </row>
     <row r="167" spans="1:2">
-      <c r="A167" s="8">
+      <c r="A167" s="6">
         <v>180142001</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -2016,7 +2020,7 @@
       </c>
     </row>
     <row r="168" spans="1:2">
-      <c r="A168" s="8">
+      <c r="A168" s="6">
         <v>180142001</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -2024,7 +2028,7 @@
       </c>
     </row>
     <row r="169" spans="1:2">
-      <c r="A169" s="8">
+      <c r="A169" s="6">
         <v>180141600</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -2032,7 +2036,7 @@
       </c>
     </row>
     <row r="170" spans="1:2">
-      <c r="A170" s="8">
+      <c r="A170" s="6">
         <v>180141600</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -2040,7 +2044,7 @@
       </c>
     </row>
     <row r="171" spans="1:2">
-      <c r="A171" s="8">
+      <c r="A171" s="6">
         <v>180141600</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -2048,7 +2052,7 @@
       </c>
     </row>
     <row r="172" spans="1:2">
-      <c r="A172" s="8" t="s">
+      <c r="A172" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -2056,7 +2060,7 @@
       </c>
     </row>
     <row r="173" spans="1:2">
-      <c r="A173" s="9">
+      <c r="A173" s="7">
         <v>180176601</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -2064,7 +2068,7 @@
       </c>
     </row>
     <row r="174" spans="1:2">
-      <c r="A174" s="9">
+      <c r="A174" s="7">
         <v>180176601</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -2072,7 +2076,7 @@
       </c>
     </row>
     <row r="175" spans="1:2">
-      <c r="A175" s="8">
+      <c r="A175" s="6">
         <v>180176500</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -2080,7 +2084,7 @@
       </c>
     </row>
     <row r="176" spans="1:2">
-      <c r="A176" s="8">
+      <c r="A176" s="6">
         <v>180176500</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -2088,7 +2092,7 @@
       </c>
     </row>
     <row r="177" spans="1:2">
-      <c r="A177" s="8">
+      <c r="A177" s="6">
         <v>180145102</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -2096,7 +2100,7 @@
       </c>
     </row>
     <row r="178" spans="1:2">
-      <c r="A178" s="8">
+      <c r="A178" s="6">
         <v>180141400</v>
       </c>
       <c r="B178" s="1" t="s">
@@ -2104,7 +2108,7 @@
       </c>
     </row>
     <row r="179" spans="1:2">
-      <c r="A179" s="8">
+      <c r="A179" s="6">
         <v>180177300</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -2112,7 +2116,7 @@
       </c>
     </row>
     <row r="180" spans="1:2">
-      <c r="A180" s="8">
+      <c r="A180" s="6">
         <v>180177300</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -2120,7 +2124,7 @@
       </c>
     </row>
     <row r="181" spans="1:2">
-      <c r="A181" s="8">
+      <c r="A181" s="6">
         <v>180177300</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -2128,7 +2132,7 @@
       </c>
     </row>
     <row r="182" spans="1:2">
-      <c r="A182" s="8">
+      <c r="A182" s="6">
         <v>180177300</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -2136,7 +2140,7 @@
       </c>
     </row>
     <row r="183" spans="1:2">
-      <c r="A183" s="8">
+      <c r="A183" s="6">
         <v>180177300</v>
       </c>
       <c r="B183" s="1" t="s">
@@ -2144,7 +2148,7 @@
       </c>
     </row>
     <row r="184" spans="1:2">
-      <c r="A184" s="8">
+      <c r="A184" s="6">
         <v>180177300</v>
       </c>
       <c r="B184" s="1" t="s">
@@ -2152,7 +2156,7 @@
       </c>
     </row>
     <row r="185" spans="1:2">
-      <c r="A185" s="8">
+      <c r="A185" s="6">
         <v>180141400</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -2160,7 +2164,7 @@
       </c>
     </row>
     <row r="186" spans="1:2">
-      <c r="A186" s="8">
+      <c r="A186" s="6">
         <v>180141400</v>
       </c>
       <c r="B186" s="1" t="s">
@@ -2168,7 +2172,7 @@
       </c>
     </row>
     <row r="187" spans="1:2">
-      <c r="A187" s="8">
+      <c r="A187" s="6">
         <v>180141400</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -2176,7 +2180,7 @@
       </c>
     </row>
     <row r="188" spans="1:2">
-      <c r="A188" s="8">
+      <c r="A188" s="6">
         <v>180141400</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -2184,7 +2188,7 @@
       </c>
     </row>
     <row r="189" spans="1:2">
-      <c r="A189" s="8">
+      <c r="A189" s="6">
         <v>180141400</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -2192,7 +2196,7 @@
       </c>
     </row>
     <row r="190" spans="1:2">
-      <c r="A190" s="8">
+      <c r="A190" s="6">
         <v>180141400</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -2200,7 +2204,7 @@
       </c>
     </row>
     <row r="191" spans="1:2">
-      <c r="A191" s="8">
+      <c r="A191" s="6">
         <v>180141400</v>
       </c>
       <c r="B191" s="1" t="s">
@@ -2208,7 +2212,7 @@
       </c>
     </row>
     <row r="192" spans="1:2">
-      <c r="A192" s="8">
+      <c r="A192" s="6">
         <v>180141400</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -2216,7 +2220,7 @@
       </c>
     </row>
     <row r="193" spans="1:2">
-      <c r="A193" s="8">
+      <c r="A193" s="6">
         <v>180141400</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -2224,7 +2228,7 @@
       </c>
     </row>
     <row r="194" spans="1:2">
-      <c r="A194" s="8">
+      <c r="A194" s="6">
         <v>180141400</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -2232,7 +2236,7 @@
       </c>
     </row>
     <row r="195" spans="1:2">
-      <c r="A195" s="8">
+      <c r="A195" s="6">
         <v>180141400</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -2240,7 +2244,7 @@
       </c>
     </row>
     <row r="196" spans="1:2">
-      <c r="A196" s="8">
+      <c r="A196" s="6">
         <v>180141400</v>
       </c>
       <c r="B196" s="1" t="s">
@@ -2248,7 +2252,7 @@
       </c>
     </row>
     <row r="197" spans="1:2">
-      <c r="A197" s="8">
+      <c r="A197" s="6">
         <v>180141400</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -2256,7 +2260,7 @@
       </c>
     </row>
     <row r="198" spans="1:2">
-      <c r="A198" s="8">
+      <c r="A198" s="6">
         <v>180142002</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -2264,7 +2268,7 @@
       </c>
     </row>
     <row r="199" spans="1:2">
-      <c r="A199" s="8">
+      <c r="A199" s="6">
         <v>180142000</v>
       </c>
       <c r="B199" s="1" t="s">
@@ -2272,7 +2276,7 @@
       </c>
     </row>
     <row r="200" spans="1:2">
-      <c r="A200" s="8">
+      <c r="A200" s="6">
         <v>180142000</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -2280,7 +2284,7 @@
       </c>
     </row>
     <row r="201" spans="1:2">
-      <c r="A201" s="8">
+      <c r="A201" s="6">
         <v>180142000</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -2288,7 +2292,7 @@
       </c>
     </row>
     <row r="202" spans="1:2">
-      <c r="A202" s="8">
+      <c r="A202" s="6">
         <v>180142000</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -2296,7 +2300,7 @@
       </c>
     </row>
     <row r="203" spans="1:2">
-      <c r="A203" s="8">
+      <c r="A203" s="6">
         <v>180142000</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -2304,7 +2308,7 @@
       </c>
     </row>
     <row r="204" spans="1:2">
-      <c r="A204" s="8">
+      <c r="A204" s="6">
         <v>180142000</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -2312,7 +2316,7 @@
       </c>
     </row>
     <row r="205" spans="1:2">
-      <c r="A205" s="8">
+      <c r="A205" s="6">
         <v>180142000</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -2320,7 +2324,7 @@
       </c>
     </row>
     <row r="206" spans="1:2">
-      <c r="A206" s="8">
+      <c r="A206" s="6">
         <v>180142000</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -2328,7 +2332,7 @@
       </c>
     </row>
     <row r="207" spans="1:2">
-      <c r="A207" s="8">
+      <c r="A207" s="6">
         <v>180142000</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -2336,7 +2340,7 @@
       </c>
     </row>
     <row r="208" spans="1:2">
-      <c r="A208" s="8">
+      <c r="A208" s="6">
         <v>180142000</v>
       </c>
       <c r="B208" s="1" t="s">
@@ -2344,7 +2348,7 @@
       </c>
     </row>
     <row r="209" spans="1:2">
-      <c r="A209" s="8" t="s">
+      <c r="A209" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B209" s="1" t="s">
@@ -2352,7 +2356,7 @@
       </c>
     </row>
     <row r="210" spans="1:2">
-      <c r="A210" s="8">
+      <c r="A210" s="6">
         <v>180176502</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -2360,7 +2364,7 @@
       </c>
     </row>
     <row r="211" spans="1:2">
-      <c r="A211" s="8">
+      <c r="A211" s="6">
         <v>180165002</v>
       </c>
       <c r="B211" s="1" t="s">
@@ -2368,7 +2372,7 @@
       </c>
     </row>
     <row r="212" spans="1:2">
-      <c r="A212" s="8">
+      <c r="A212" s="6">
         <v>180165002</v>
       </c>
       <c r="B212" s="1" t="s">
@@ -2376,7 +2380,7 @@
       </c>
     </row>
     <row r="213" spans="1:2">
-      <c r="A213" s="8">
+      <c r="A213" s="6">
         <v>180165002</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -2384,7 +2388,7 @@
       </c>
     </row>
     <row r="214" spans="1:2">
-      <c r="A214" s="8">
+      <c r="A214" s="6">
         <v>180141500</v>
       </c>
       <c r="B214" s="1" t="s">
@@ -2392,7 +2396,7 @@
       </c>
     </row>
     <row r="215" spans="1:2">
-      <c r="A215" s="8">
+      <c r="A215" s="6">
         <v>180141500</v>
       </c>
       <c r="B215" s="1" t="s">
@@ -2400,7 +2404,7 @@
       </c>
     </row>
     <row r="216" spans="1:2">
-      <c r="A216" s="8">
+      <c r="A216" s="6">
         <v>180141500</v>
       </c>
       <c r="B216" s="1" t="s">
@@ -2408,7 +2412,7 @@
       </c>
     </row>
     <row r="217" spans="1:2">
-      <c r="A217" s="8">
+      <c r="A217" s="6">
         <v>180141500</v>
       </c>
       <c r="B217" s="1" t="s">
@@ -2416,7 +2420,7 @@
       </c>
     </row>
     <row r="218" spans="1:2">
-      <c r="A218" s="8">
+      <c r="A218" s="6">
         <v>180141500</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -2424,7 +2428,7 @@
       </c>
     </row>
     <row r="219" spans="1:2">
-      <c r="A219" s="8">
+      <c r="A219" s="6">
         <v>180141500</v>
       </c>
       <c r="B219" s="1" t="s">
@@ -2432,7 +2436,7 @@
       </c>
     </row>
     <row r="220" spans="1:2">
-      <c r="A220" s="8">
+      <c r="A220" s="6">
         <v>180141500</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -2440,7 +2444,7 @@
       </c>
     </row>
     <row r="221" spans="1:2">
-      <c r="A221" s="8">
+      <c r="A221" s="6">
         <v>180141500</v>
       </c>
       <c r="B221" s="1" t="s">
@@ -2448,7 +2452,7 @@
       </c>
     </row>
     <row r="222" spans="1:2">
-      <c r="A222" s="8">
+      <c r="A222" s="6">
         <v>180141500</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -2456,7 +2460,7 @@
       </c>
     </row>
     <row r="223" spans="1:2">
-      <c r="A223" s="8">
+      <c r="A223" s="6">
         <v>180141500</v>
       </c>
       <c r="B223" s="1" t="s">
@@ -2464,7 +2468,7 @@
       </c>
     </row>
     <row r="224" spans="1:2">
-      <c r="A224" s="8">
+      <c r="A224" s="6">
         <v>180141500</v>
       </c>
       <c r="B224" s="1" t="s">
@@ -2472,7 +2476,7 @@
       </c>
     </row>
     <row r="225" spans="1:2">
-      <c r="A225" s="8">
+      <c r="A225" s="6">
         <v>180141500</v>
       </c>
       <c r="B225" s="1" t="s">
@@ -2480,7 +2484,7 @@
       </c>
     </row>
     <row r="226" spans="1:2">
-      <c r="A226" s="8">
+      <c r="A226" s="6">
         <v>180141500</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -2488,7 +2492,7 @@
       </c>
     </row>
     <row r="227" spans="1:2">
-      <c r="A227" s="8">
+      <c r="A227" s="6">
         <v>180141500</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -2496,7 +2500,7 @@
       </c>
     </row>
     <row r="228" spans="1:2">
-      <c r="A228" s="8">
+      <c r="A228" s="6">
         <v>180141500</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -2504,7 +2508,7 @@
       </c>
     </row>
     <row r="229" spans="1:2">
-      <c r="A229" s="8">
+      <c r="A229" s="6">
         <v>180141401</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -2512,7 +2516,7 @@
       </c>
     </row>
     <row r="230" spans="1:2">
-      <c r="A230" s="8">
+      <c r="A230" s="6">
         <v>180141401</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -2520,7 +2524,7 @@
       </c>
     </row>
     <row r="231" spans="1:2">
-      <c r="A231" s="8">
+      <c r="A231" s="6">
         <v>180141401</v>
       </c>
       <c r="B231" s="1" t="s">
@@ -2528,7 +2532,7 @@
       </c>
     </row>
     <row r="232" spans="1:2">
-      <c r="A232" s="8">
+      <c r="A232" s="6">
         <v>180141300</v>
       </c>
       <c r="B232" s="1" t="s">
@@ -2536,7 +2540,7 @@
       </c>
     </row>
     <row r="233" spans="1:2">
-      <c r="A233" s="8">
+      <c r="A233" s="6">
         <v>180146700</v>
       </c>
       <c r="B233" s="1" t="s">
@@ -2544,7 +2548,7 @@
       </c>
     </row>
     <row r="234" spans="1:2">
-      <c r="A234" s="8">
+      <c r="A234" s="6">
         <v>180146700</v>
       </c>
       <c r="B234" s="1" t="s">
@@ -2552,7 +2556,7 @@
       </c>
     </row>
     <row r="235" spans="1:2">
-      <c r="A235" s="8">
+      <c r="A235" s="6">
         <v>180146700</v>
       </c>
       <c r="B235" s="1" t="s">
@@ -2560,7 +2564,7 @@
       </c>
     </row>
     <row r="236" spans="1:2">
-      <c r="A236" s="8">
+      <c r="A236" s="6">
         <v>180146700</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -2568,7 +2572,7 @@
       </c>
     </row>
     <row r="237" spans="1:2">
-      <c r="A237" s="8">
+      <c r="A237" s="6">
         <v>180146700</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -2576,7 +2580,7 @@
       </c>
     </row>
     <row r="238" spans="1:2">
-      <c r="A238" s="8">
+      <c r="A238" s="6">
         <v>180146700</v>
       </c>
       <c r="B238" s="1" t="s">
@@ -2584,7 +2588,7 @@
       </c>
     </row>
     <row r="239" spans="1:2">
-      <c r="A239" s="8">
+      <c r="A239" s="6">
         <v>180146700</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -2592,7 +2596,7 @@
       </c>
     </row>
     <row r="240" spans="1:2">
-      <c r="A240" s="8">
+      <c r="A240" s="6">
         <v>180146700</v>
       </c>
       <c r="B240" s="1" t="s">
@@ -2600,7 +2604,7 @@
       </c>
     </row>
     <row r="241" spans="1:2">
-      <c r="A241" s="8">
+      <c r="A241" s="6">
         <v>180176800</v>
       </c>
       <c r="B241" s="1" t="s">
@@ -2608,7 +2612,7 @@
       </c>
     </row>
     <row r="242" spans="1:2">
-      <c r="A242" s="8">
+      <c r="A242" s="6">
         <v>180141100</v>
       </c>
       <c r="B242" s="1" t="s">
@@ -2616,7 +2620,7 @@
       </c>
     </row>
     <row r="243" spans="1:2">
-      <c r="A243" s="8">
+      <c r="A243" s="6">
         <v>180145101</v>
       </c>
       <c r="B243" s="1" t="s">
@@ -2624,7 +2628,7 @@
       </c>
     </row>
     <row r="244" spans="1:2">
-      <c r="A244" s="8">
+      <c r="A244" s="6">
         <v>180145101</v>
       </c>
       <c r="B244" s="1" t="s">
@@ -2632,7 +2636,7 @@
       </c>
     </row>
     <row r="245" spans="1:2">
-      <c r="A245" s="8">
+      <c r="A245" s="6">
         <v>180177800</v>
       </c>
       <c r="B245" s="1" t="s">
@@ -2640,7 +2644,7 @@
       </c>
     </row>
     <row r="246" spans="1:2">
-      <c r="A246" s="8">
+      <c r="A246" s="6">
         <v>180177800</v>
       </c>
       <c r="B246" s="1" t="s">
@@ -2648,7 +2652,7 @@
       </c>
     </row>
     <row r="247" spans="1:2">
-      <c r="A247" s="8">
+      <c r="A247" s="6">
         <v>180177800</v>
       </c>
       <c r="B247" s="1" t="s">
@@ -2656,7 +2660,7 @@
       </c>
     </row>
     <row r="248" spans="1:2">
-      <c r="A248" s="8">
+      <c r="A248" s="6">
         <v>180177800</v>
       </c>
       <c r="B248" s="1" t="s">
@@ -2664,7 +2668,7 @@
       </c>
     </row>
     <row r="249" spans="1:2">
-      <c r="A249" s="8">
+      <c r="A249" s="6">
         <v>180177800</v>
       </c>
       <c r="B249" s="1" t="s">
@@ -2672,7 +2676,7 @@
       </c>
     </row>
     <row r="250" spans="1:2">
-      <c r="A250" s="8">
+      <c r="A250" s="6">
         <v>180177800</v>
       </c>
       <c r="B250" s="1" t="s">
@@ -2680,7 +2684,7 @@
       </c>
     </row>
     <row r="251" spans="1:2">
-      <c r="A251" s="8">
+      <c r="A251" s="6">
         <v>180141201</v>
       </c>
       <c r="B251" s="1" t="s">
@@ -2688,7 +2692,7 @@
       </c>
     </row>
     <row r="252" spans="1:2">
-      <c r="A252" s="8">
+      <c r="A252" s="6">
         <v>180183000</v>
       </c>
       <c r="B252" s="1" t="s">
@@ -2696,7 +2700,7 @@
       </c>
     </row>
     <row r="253" spans="1:2">
-      <c r="A253" s="8">
+      <c r="A253" s="6">
         <v>180183000</v>
       </c>
       <c r="B253" s="1" t="s">
@@ -2704,7 +2708,7 @@
       </c>
     </row>
     <row r="254" spans="1:2">
-      <c r="A254" s="8">
+      <c r="A254" s="6">
         <v>180183000</v>
       </c>
       <c r="B254" s="1" t="s">
@@ -2712,7 +2716,7 @@
       </c>
     </row>
     <row r="255" spans="1:2">
-      <c r="A255" s="8">
+      <c r="A255" s="6">
         <v>180183000</v>
       </c>
       <c r="B255" s="2" t="s">
@@ -2720,7 +2724,7 @@
       </c>
     </row>
     <row r="256" spans="1:2">
-      <c r="A256" s="8">
+      <c r="A256" s="6">
         <v>180183000</v>
       </c>
       <c r="B256" s="1" t="s">
@@ -2728,7 +2732,7 @@
       </c>
     </row>
     <row r="257" spans="1:2">
-      <c r="A257" s="8">
+      <c r="A257" s="6">
         <v>180183000</v>
       </c>
       <c r="B257" s="2" t="s">
@@ -2736,7 +2740,7 @@
       </c>
     </row>
     <row r="258" spans="1:2">
-      <c r="A258" s="8">
+      <c r="A258" s="6">
         <v>180146600</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -2744,7 +2748,7 @@
       </c>
     </row>
     <row r="259" spans="1:2">
-      <c r="A259" s="8">
+      <c r="A259" s="6">
         <v>180146600</v>
       </c>
       <c r="B259" s="1" t="s">
@@ -2752,7 +2756,7 @@
       </c>
     </row>
     <row r="260" spans="1:2">
-      <c r="A260" s="8">
+      <c r="A260" s="6">
         <v>180146600</v>
       </c>
       <c r="B260" s="1" t="s">
@@ -2760,7 +2764,7 @@
       </c>
     </row>
     <row r="261" spans="1:2">
-      <c r="A261" s="8">
+      <c r="A261" s="6">
         <v>180146600</v>
       </c>
       <c r="B261" s="1" t="s">
@@ -2768,7 +2772,7 @@
       </c>
     </row>
     <row r="262" spans="1:2">
-      <c r="A262" s="8">
+      <c r="A262" s="6">
         <v>180146600</v>
       </c>
       <c r="B262" s="1" t="s">
@@ -2776,7 +2780,7 @@
       </c>
     </row>
     <row r="263" spans="1:2">
-      <c r="A263" s="8">
+      <c r="A263" s="6">
         <v>180146600</v>
       </c>
       <c r="B263" s="1" t="s">
@@ -2784,7 +2788,7 @@
       </c>
     </row>
     <row r="264" spans="1:2">
-      <c r="A264" s="8">
+      <c r="A264" s="6">
         <v>180146600</v>
       </c>
       <c r="B264" s="1" t="s">
@@ -2792,7 +2796,7 @@
       </c>
     </row>
     <row r="265" spans="1:2">
-      <c r="A265" s="8">
+      <c r="A265" s="6">
         <v>180041101</v>
       </c>
       <c r="B265" s="1" t="s">
@@ -2800,7 +2804,7 @@
       </c>
     </row>
     <row r="266" spans="1:2">
-      <c r="A266" s="8">
+      <c r="A266" s="6">
         <v>180041101</v>
       </c>
       <c r="B266" s="1" t="s">
@@ -2808,7 +2812,7 @@
       </c>
     </row>
     <row r="267" spans="1:2">
-      <c r="A267" s="8">
+      <c r="A267" s="6">
         <v>180176600</v>
       </c>
       <c r="B267" s="1" t="s">
@@ -2816,7 +2820,7 @@
       </c>
     </row>
     <row r="268" spans="1:2">
-      <c r="A268" s="8">
+      <c r="A268" s="6">
         <v>180176600</v>
       </c>
       <c r="B268" s="1" t="s">
@@ -2824,7 +2828,7 @@
       </c>
     </row>
     <row r="269" spans="1:2">
-      <c r="A269" s="8">
+      <c r="A269" s="6">
         <v>180176600</v>
       </c>
       <c r="B269" s="1" t="s">
@@ -2832,7 +2836,7 @@
       </c>
     </row>
     <row r="270" spans="1:2">
-      <c r="A270" s="8">
+      <c r="A270" s="6">
         <v>180176600</v>
       </c>
       <c r="B270" s="1" t="s">
@@ -2840,7 +2844,7 @@
       </c>
     </row>
     <row r="271" spans="1:2">
-      <c r="A271" s="8">
+      <c r="A271" s="6">
         <v>180146701</v>
       </c>
       <c r="B271" s="1" t="s">
@@ -2848,7 +2852,7 @@
       </c>
     </row>
     <row r="272" spans="1:2">
-      <c r="A272" s="8">
+      <c r="A272" s="6">
         <v>180146701</v>
       </c>
       <c r="B272" s="1" t="s">
@@ -2856,7 +2860,7 @@
       </c>
     </row>
     <row r="273" spans="1:2">
-      <c r="A273" s="8">
+      <c r="A273" s="6">
         <v>180146701</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -2864,7 +2868,7 @@
       </c>
     </row>
     <row r="274" spans="1:2">
-      <c r="A274" s="8">
+      <c r="A274" s="6">
         <v>180032000</v>
       </c>
       <c r="B274" s="1" t="s">
@@ -2872,7 +2876,7 @@
       </c>
     </row>
     <row r="275" spans="1:2">
-      <c r="A275" s="8">
+      <c r="A275" s="6">
         <v>180032000</v>
       </c>
       <c r="B275" s="1" t="s">
@@ -2880,7 +2884,7 @@
       </c>
     </row>
     <row r="276" spans="1:2">
-      <c r="A276" s="8">
+      <c r="A276" s="6">
         <v>180032000</v>
       </c>
       <c r="B276" s="1" t="s">
@@ -2888,7 +2892,7 @@
       </c>
     </row>
     <row r="277" spans="1:2">
-      <c r="A277" s="8">
+      <c r="A277" s="6">
         <v>180032000</v>
       </c>
       <c r="B277" s="1" t="s">
@@ -2896,7 +2900,7 @@
       </c>
     </row>
     <row r="278" spans="1:2">
-      <c r="A278" s="8">
+      <c r="A278" s="6">
         <v>180032000</v>
       </c>
       <c r="B278" s="1" t="s">
@@ -2904,7 +2908,7 @@
       </c>
     </row>
     <row r="279" spans="1:2">
-      <c r="A279" s="8">
+      <c r="A279" s="6">
         <v>180032000</v>
       </c>
       <c r="B279" s="1" t="s">
@@ -2912,7 +2916,7 @@
       </c>
     </row>
     <row r="280" spans="1:2">
-      <c r="A280" s="8">
+      <c r="A280" s="6">
         <v>180032000</v>
       </c>
       <c r="B280" s="1" t="s">
@@ -2920,7 +2924,7 @@
       </c>
     </row>
     <row r="281" spans="1:2">
-      <c r="A281" s="8">
+      <c r="A281" s="6">
         <v>180032000</v>
       </c>
       <c r="B281" s="1" t="s">
@@ -2928,7 +2932,7 @@
       </c>
     </row>
     <row r="282" spans="1:2">
-      <c r="A282" s="8">
+      <c r="A282" s="6">
         <v>180032000</v>
       </c>
       <c r="B282" s="1" t="s">
@@ -2936,7 +2940,7 @@
       </c>
     </row>
     <row r="283" spans="1:2">
-      <c r="A283" s="8">
+      <c r="A283" s="6">
         <v>180032000</v>
       </c>
       <c r="B283" s="1" t="s">
@@ -2944,7 +2948,7 @@
       </c>
     </row>
     <row r="284" spans="1:2">
-      <c r="A284" s="8">
+      <c r="A284" s="6">
         <v>180032000</v>
       </c>
       <c r="B284" s="1" t="s">
@@ -2952,7 +2956,7 @@
       </c>
     </row>
     <row r="285" spans="1:2">
-      <c r="A285" s="8">
+      <c r="A285" s="6">
         <v>180177100</v>
       </c>
       <c r="B285" s="1" t="s">
@@ -2960,7 +2964,7 @@
       </c>
     </row>
     <row r="286" spans="1:2">
-      <c r="A286" s="8">
+      <c r="A286" s="6">
         <v>180177100</v>
       </c>
       <c r="B286" s="1" t="s">
@@ -2968,7 +2972,7 @@
       </c>
     </row>
     <row r="287" spans="1:2">
-      <c r="A287" s="8">
+      <c r="A287" s="6">
         <v>180177100</v>
       </c>
       <c r="B287" s="1" t="s">
@@ -2976,7 +2980,7 @@
       </c>
     </row>
     <row r="288" spans="1:2">
-      <c r="A288" s="8">
+      <c r="A288" s="6">
         <v>180177100</v>
       </c>
       <c r="B288" s="1" t="s">
@@ -2984,7 +2988,7 @@
       </c>
     </row>
     <row r="289" spans="1:2">
-      <c r="A289" s="8">
+      <c r="A289" s="6">
         <v>180177100</v>
       </c>
       <c r="B289" s="1" t="s">
@@ -2992,7 +2996,7 @@
       </c>
     </row>
     <row r="290" spans="1:2">
-      <c r="A290" s="8">
+      <c r="A290" s="6">
         <v>180177100</v>
       </c>
       <c r="B290" s="1" t="s">
@@ -3000,7 +3004,7 @@
       </c>
     </row>
     <row r="291" spans="1:2">
-      <c r="A291" s="8">
+      <c r="A291" s="6">
         <v>180146702</v>
       </c>
       <c r="B291" s="1" t="s">
@@ -3008,7 +3012,7 @@
       </c>
     </row>
     <row r="292" spans="1:2">
-      <c r="A292" s="8">
+      <c r="A292" s="6">
         <v>180146702</v>
       </c>
       <c r="B292" s="1" t="s">
@@ -3016,7 +3020,7 @@
       </c>
     </row>
     <row r="293" spans="1:2">
-      <c r="A293" s="8">
+      <c r="A293" s="6">
         <v>180146702</v>
       </c>
       <c r="B293" s="1" t="s">
@@ -3024,7 +3028,7 @@
       </c>
     </row>
     <row r="294" spans="1:2">
-      <c r="A294" s="8">
+      <c r="A294" s="6">
         <v>180141501</v>
       </c>
       <c r="B294" s="1" t="s">
@@ -3032,7 +3036,7 @@
       </c>
     </row>
     <row r="295" spans="1:2">
-      <c r="A295" s="8">
+      <c r="A295" s="6">
         <v>180141501</v>
       </c>
       <c r="B295" s="1" t="s">
@@ -3040,7 +3044,7 @@
       </c>
     </row>
     <row r="296" spans="1:2">
-      <c r="A296" s="10">
+      <c r="A296" s="8">
         <v>180141501</v>
       </c>
       <c r="B296" s="4" t="s">
@@ -3048,7 +3052,7 @@
       </c>
     </row>
     <row r="297" spans="1:2">
-      <c r="A297" s="11">
+      <c r="A297" s="9">
         <v>180107900</v>
       </c>
       <c r="B297" s="5" t="s">
@@ -3056,7 +3060,7 @@
       </c>
     </row>
     <row r="298" spans="1:2">
-      <c r="A298" s="11">
+      <c r="A298" s="9">
         <v>180107900</v>
       </c>
       <c r="B298" s="5" t="s">
@@ -3064,7 +3068,7 @@
       </c>
     </row>
     <row r="299" spans="1:2">
-      <c r="A299" s="11">
+      <c r="A299" s="9">
         <v>180107900</v>
       </c>
       <c r="B299" s="5" t="s">
@@ -3072,7 +3076,7 @@
       </c>
     </row>
     <row r="300" spans="1:2">
-      <c r="A300" s="11">
+      <c r="A300" s="9">
         <v>180069800</v>
       </c>
       <c r="B300" s="5" t="s">
@@ -3080,7 +3084,7 @@
       </c>
     </row>
     <row r="301" spans="1:2">
-      <c r="A301" s="11">
+      <c r="A301" s="9">
         <v>180069800</v>
       </c>
       <c r="B301" s="5" t="s">
@@ -3088,7 +3092,7 @@
       </c>
     </row>
     <row r="302" spans="1:2">
-      <c r="A302" s="11">
+      <c r="A302" s="9">
         <v>180069800</v>
       </c>
       <c r="B302" s="5" t="s">
@@ -3096,7 +3100,7 @@
       </c>
     </row>
     <row r="303" spans="1:2">
-      <c r="A303" s="11">
+      <c r="A303" s="9">
         <v>180086700</v>
       </c>
       <c r="B303" s="5" t="s">
@@ -3104,7 +3108,7 @@
       </c>
     </row>
     <row r="304" spans="1:2">
-      <c r="A304" s="11">
+      <c r="A304" s="9">
         <v>180086700</v>
       </c>
       <c r="B304" s="5" t="s">
@@ -3112,7 +3116,7 @@
       </c>
     </row>
     <row r="305" spans="1:2">
-      <c r="A305" s="11">
+      <c r="A305" s="9">
         <v>180086700</v>
       </c>
       <c r="B305" s="5" t="s">
@@ -3120,7 +3124,7 @@
       </c>
     </row>
     <row r="306" spans="1:2">
-      <c r="A306" s="11">
+      <c r="A306" s="9">
         <v>180155500</v>
       </c>
       <c r="B306" s="5" t="s">
@@ -3128,7 +3132,7 @@
       </c>
     </row>
     <row r="307" spans="1:2">
-      <c r="A307" s="11">
+      <c r="A307" s="9">
         <v>180019800</v>
       </c>
       <c r="B307" s="5" t="s">
@@ -3136,7 +3140,7 @@
       </c>
     </row>
     <row r="308" spans="1:2">
-      <c r="A308" s="11">
+      <c r="A308" s="9">
         <v>180019800</v>
       </c>
       <c r="B308" s="5" t="s">
@@ -3144,7 +3148,7 @@
       </c>
     </row>
     <row r="309" spans="1:2">
-      <c r="A309" s="11">
+      <c r="A309" s="9">
         <v>180019800</v>
       </c>
       <c r="B309" s="5" t="s">
@@ -3152,7 +3156,7 @@
       </c>
     </row>
     <row r="310" spans="1:2">
-      <c r="A310" s="11">
+      <c r="A310" s="9">
         <v>180114400</v>
       </c>
       <c r="B310" s="5" t="s">
@@ -3160,7 +3164,7 @@
       </c>
     </row>
     <row r="311" spans="1:2">
-      <c r="A311" s="11">
+      <c r="A311" s="9">
         <v>180114400</v>
       </c>
       <c r="B311" s="5" t="s">
@@ -3168,7 +3172,7 @@
       </c>
     </row>
     <row r="312" spans="1:2">
-      <c r="A312" s="11">
+      <c r="A312" s="9">
         <v>180114400</v>
       </c>
       <c r="B312" s="5" t="s">
@@ -3176,7 +3180,7 @@
       </c>
     </row>
     <row r="313" spans="1:2">
-      <c r="A313" s="11">
+      <c r="A313" s="9">
         <v>180114400</v>
       </c>
       <c r="B313" s="5" t="s">
@@ -3184,7 +3188,7 @@
       </c>
     </row>
     <row r="314" spans="1:2">
-      <c r="A314" s="11">
+      <c r="A314" s="9">
         <v>180114400</v>
       </c>
       <c r="B314" s="5" t="s">
@@ -3192,7 +3196,7 @@
       </c>
     </row>
     <row r="315" spans="1:2">
-      <c r="A315" s="11">
+      <c r="A315" s="9">
         <v>180114400</v>
       </c>
       <c r="B315" s="5" t="s">
@@ -3200,7 +3204,7 @@
       </c>
     </row>
     <row r="316" spans="1:2">
-      <c r="A316" s="11">
+      <c r="A316" s="9">
         <v>180185200</v>
       </c>
       <c r="B316" s="5" t="s">
@@ -3208,7 +3212,7 @@
       </c>
     </row>
     <row r="317" spans="1:2">
-      <c r="A317" s="11">
+      <c r="A317" s="9">
         <v>180185200</v>
       </c>
       <c r="B317" s="5" t="s">
@@ -3216,7 +3220,7 @@
       </c>
     </row>
     <row r="318" spans="1:2">
-      <c r="A318" s="11">
+      <c r="A318" s="9">
         <v>180185200</v>
       </c>
       <c r="B318" s="5" t="s">
@@ -3224,7 +3228,7 @@
       </c>
     </row>
     <row r="319" spans="1:2">
-      <c r="A319" s="11">
+      <c r="A319" s="9">
         <v>180114000</v>
       </c>
       <c r="B319" s="5" t="s">
@@ -3232,7 +3236,7 @@
       </c>
     </row>
     <row r="320" spans="1:2">
-      <c r="A320" s="11">
+      <c r="A320" s="9">
         <v>180114000</v>
       </c>
       <c r="B320" s="5" t="s">
@@ -3240,7 +3244,7 @@
       </c>
     </row>
     <row r="321" spans="1:2">
-      <c r="A321" s="11">
+      <c r="A321" s="9">
         <v>180114000</v>
       </c>
       <c r="B321" s="5" t="s">
@@ -3248,7 +3252,7 @@
       </c>
     </row>
     <row r="322" spans="1:2">
-      <c r="A322" s="11">
+      <c r="A322" s="9">
         <v>180114000</v>
       </c>
       <c r="B322" s="5" t="s">
@@ -3256,7 +3260,7 @@
       </c>
     </row>
     <row r="323" spans="1:2">
-      <c r="A323" s="11">
+      <c r="A323" s="9">
         <v>180114000</v>
       </c>
       <c r="B323" s="5" t="s">
@@ -3264,7 +3268,7 @@
       </c>
     </row>
     <row r="324" spans="1:2">
-      <c r="A324" s="11">
+      <c r="A324" s="9">
         <v>180114000</v>
       </c>
       <c r="B324" s="5" t="s">
@@ -3272,7 +3276,7 @@
       </c>
     </row>
     <row r="325" spans="1:2">
-      <c r="A325" s="11">
+      <c r="A325" s="9">
         <v>180155500</v>
       </c>
       <c r="B325" s="5" t="s">
@@ -3280,38 +3284,31 @@
       </c>
     </row>
     <row r="326" spans="1:2">
-      <c r="A326" s="12"/>
-      <c r="B326" s="7"/>
+      <c r="A326" s="11">
+        <v>180146602</v>
+      </c>
+      <c r="B326" s="12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="327" spans="1:2">
-      <c r="A327" s="12"/>
-      <c r="B327" s="6"/>
+      <c r="A327" s="11">
+        <v>180146602</v>
+      </c>
+      <c r="B327" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="328" spans="1:2">
-      <c r="A328" s="8">
+      <c r="A328" s="11">
         <v>180146602</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2">
-      <c r="A329" s="8">
-        <v>180146602</v>
-      </c>
-      <c r="B329" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2">
-      <c r="A330" s="8">
-        <v>180146602</v>
-      </c>
-      <c r="B330" s="1" t="s">
+      <c r="B328" s="12" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nuevos registros escuelas tecnicas
</commit_message>
<xml_diff>
--- a/src/main/resources/superior.xlsx
+++ b/src/main/resources/superior.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="119">
   <si>
     <t>Tecnicatura Superior Agente Sanitario y Promotor de la Salud</t>
   </si>
@@ -273,13 +273,121 @@
   </si>
   <si>
     <t>Tecnicatura Superior en Comunicación Multimedial</t>
+  </si>
+  <si>
+    <t>Mecánico de Motos</t>
+  </si>
+  <si>
+    <t>Operador en Informática para la Administración y Gestión</t>
+  </si>
+  <si>
+    <t>Cocinero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizacón y Gestión </t>
+  </si>
+  <si>
+    <t>Auxiliar en Const en Seco c Comp Livianos</t>
+  </si>
+  <si>
+    <t>armador de Paneles y Cielorrasos de Placas de Yeso</t>
+  </si>
+  <si>
+    <t>Auxiliar en Instalaciones Eléctricas Domiciliarias</t>
+  </si>
+  <si>
+    <t>Montador Electricista Domiciliario</t>
+  </si>
+  <si>
+    <t>Soldador Básico</t>
+  </si>
+  <si>
+    <t>Albañil</t>
+  </si>
+  <si>
+    <t>Auxiliar en Instalaciones sanitarias y de gas domiciliarias</t>
+  </si>
+  <si>
+    <t>Montador de Instalaciones  Sanitarias  Domiciliarias</t>
+  </si>
+  <si>
+    <t>Electricista Industrial</t>
+  </si>
+  <si>
+    <t>Reparador Electrónico Básico</t>
+  </si>
+  <si>
+    <t>Reparador de Audio y Video Digital</t>
+  </si>
+  <si>
+    <t>Tornero</t>
+  </si>
+  <si>
+    <t>Fresador</t>
+  </si>
+  <si>
+    <t>Auxiliar Mecánico de Refrigeración</t>
+  </si>
+  <si>
+    <t>Bobinador de máquinas eléctricas</t>
+  </si>
+  <si>
+    <t>Mecánico en Refrigeracion en Inmuebles</t>
+  </si>
+  <si>
+    <t>Electricista de Automotores</t>
+  </si>
+  <si>
+    <t>Auxiliar Mecánico de motores Diesel</t>
+  </si>
+  <si>
+    <t>Auxiliar Mecánico en Motores Nafteros</t>
+  </si>
+  <si>
+    <t>Auxiliar  de peluquería</t>
+  </si>
+  <si>
+    <t>Carpintero de Banco</t>
+  </si>
+  <si>
+    <t>Herrero</t>
+  </si>
+  <si>
+    <t>Operador de Máquinas para la Confección de Indumentaria</t>
+  </si>
+  <si>
+    <t>Modista/o</t>
+  </si>
+  <si>
+    <t>Auxiliar en Construcciones</t>
+  </si>
+  <si>
+    <t>Auxiliar en Inst Sanit y de Gas Domic</t>
+  </si>
+  <si>
+    <t>Montador domcilirio de gas</t>
+  </si>
+  <si>
+    <t>Electricista en Inmuebles</t>
+  </si>
+  <si>
+    <t>Peluquero/a</t>
+  </si>
+  <si>
+    <t>Panadero</t>
+  </si>
+  <si>
+    <t>Pastelero</t>
+  </si>
+  <si>
+    <t>Reparador de PC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +408,23 @@
       <color rgb="FF000000"/>
       <name val="PT Sans"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +437,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -351,11 +480,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -390,6 +575,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B328"/>
+  <dimension ref="A1:B389"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="A326" sqref="A326:B328"/>
+      <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3299,12 +3517,500 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" ht="15.75" thickBot="1">
       <c r="A328" s="11">
         <v>180146602</v>
       </c>
       <c r="B328" s="12" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A329" s="13">
+        <v>180014000</v>
+      </c>
+      <c r="B329" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A330" s="13">
+        <v>180014000</v>
+      </c>
+      <c r="B330" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A331" s="13">
+        <v>180014000</v>
+      </c>
+      <c r="B331" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A332" s="13">
+        <v>180014000</v>
+      </c>
+      <c r="B332" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A333" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B333" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A334" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B334" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A335" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B335" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A336" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B336" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A337" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B337" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A338" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B338" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A339" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B339" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A340" s="18">
+        <v>180041700</v>
+      </c>
+      <c r="B340" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A341" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B341" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A342" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B342" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A343" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B343" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A344" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B344" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A345" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B345" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A346" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B346" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A347" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B347" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A348" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B348" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A349" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B349" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A350" s="18">
+        <v>180082000</v>
+      </c>
+      <c r="B350" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A351" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B351" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A352" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B352" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A353" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B353" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A354" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B354" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A355" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B355" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A356" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B356" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A357" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B357" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A358" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B358" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A359" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B359" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A360" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B360" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A361" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B361" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A362" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B362" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A363" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B363" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A364" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B364" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A365" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B365" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A366" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B366" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A367" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B367" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A368" s="20">
+        <v>180140400</v>
+      </c>
+      <c r="B368" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A369" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B369" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A370" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B370" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A371" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B371" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A372" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B372" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A373" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B373" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A374" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B374" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A375" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B375" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A376" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B376" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A377" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B377" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A378" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B378" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A379" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B379" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A380" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B380" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A381" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B381" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A382" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B382" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A383" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B383" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A384" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B384" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A385" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B385" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A386" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B386" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A387" s="20">
+        <v>180142300</v>
+      </c>
+      <c r="B387" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A388" s="22">
+        <v>180155100</v>
+      </c>
+      <c r="B388" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="22">
+        <v>180164400</v>
+      </c>
+      <c r="B389" s="23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>